<commit_message>
Restruktur and add readme
</commit_message>
<xml_diff>
--- a/list_files.xlsx
+++ b/list_files.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,224 +454,549 @@
           <t>Links</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>jenjang</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>halaman 10</t>
+          <t>halaman 7</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Sekolah halaman 10</t>
+          <t>Sekolah halaman 7</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1uxuDUE4GTuqdh6ypo_TfCT4UHsJbQZDo</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1miERX46gsuFVa9PNsL56scoiK4CWqRXC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>8</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>halaman 2</t>
+          <t>halaman 8</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Sekolah halaman 2</t>
+          <t>Sekolah halaman 8</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1cDcceu27VWTuLDVaeNwHkx9kEVr907Rf</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1OtbMjfalpo7DtdUQuG31pQvwRMY2OhJO</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>halaman 5</t>
+          <t>halaman 3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Sekolah halaman 5</t>
+          <t>Sekolah halaman 3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1mLrCFAHUjXS_oQIE3quOP9w8QFUdIMmh</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1WFM9dqVtzajNbJOG19HpBHmbaVsq90AA</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>halaman 3</t>
+          <t>halaman 5</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Sekolah halaman 3</t>
+          <t>Sekolah halaman 5</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1Hw6akmhPYBhpDgpxGr2ZhTrXIrgpaqkc</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1-oE_Tk-l5mOIKeVMggnK2kDI6u2sM8e8</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>halaman 1</t>
+          <t>halaman 4</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Sekolah halaman 1</t>
+          <t>Sekolah halaman 4</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1u1Nqee8cDlpddx2U8tF56ggkC_wLKSTY</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1fuqe94jS22cc5ImQiWnKnE7VyhI0A07r</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>halaman 4</t>
+          <t>halaman 9</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Sekolah halaman 4</t>
+          <t>Sekolah halaman 9</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1AdTygcV0XZaHgXxMWUuqrMC29BtH7W3Y</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1ExkfsNsL4bpsPn9sfYb5wJbzjv3jJ9yC</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>halaman 8</t>
+          <t>halaman 2</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Sekolah halaman 8</t>
+          <t>Sekolah halaman 2</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=18akpIITCB1Ymr884kBkzfLiGzrgKvYs0</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=16saOCe8EbbfEa_crnCcjdw33RR4szcZ-</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>halaman 6</t>
+          <t>halaman 1</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sekolah halaman 6</t>
+          <t>Sekolah halaman 1</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1DQqCR3xibUlhKAI-2soWaKqkmDT3pIhK</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1xEeSeeEdtMcjGtSmMeCR8yuIUQ0ziuO_</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>halaman 9</t>
+          <t>halaman 10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sekolah halaman 9</t>
+          <t>Sekolah halaman 10</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=1aT9JysxdJmplqEmvDZrXkh-Ss5xdFFoe</t>
+          <t>https://drive.google.com/uc?export=download&amp;id=1EiOS6kSkhNZC1aGF4IlW3X36OukCZw2v</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>TK</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>halaman 6</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 6</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1edRJqm7X0ciMC7sm79Tq1Z21eIMyHNJG</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>TK</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>halaman 1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 1</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1S3GHTIc8fbrVRKKrxHgtV3AvgTn6aUcA</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>halaman 4</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 4</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1y9Y6P2eo4Xs53I7yp1-FPJ_41u521Cq3</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>halaman 3</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 3</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1PAzC3xS_s7nEjtn4mdUilIXGyz3BdFUl</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>halaman 2</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 2</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1ZL7kauqEAHHD39tLnBWeHKiKE5foKx7i</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>halaman 8</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 8</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1WSYYsSDqWLLlEUJvG3cstsCvAFEXasMT</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>halaman 5</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 5</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1sRvxyZXMHYb7Sg-cal1g1EURK3eY7JFl</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>halaman 6</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 6</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1H4RGipajL8A7VeeTHm0o_UK3QG6XNIhv</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>halaman 9</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 9</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1jSTtr8O5jAynjbfiXobKoSujXf-L0IwW</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>7</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>halaman 7</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>Sekolah halaman 7</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>https://drive.google.com/uc?export=download&amp;id=19ceWqGt6hl88bpgbMif7j68UXvm6WM5r</t>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=13HDcDzuPq3CW9XEzI_rXDzjmd3yHHFFj</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>halaman 10</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Sekolah halaman 10</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>https://drive.google.com/uc?export=download&amp;id=1F9r-UU8fvMAbgZBAs41RKipC8ra5AyCj</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>SD</t>
         </is>
       </c>
     </row>

</xml_diff>